<commit_message>
Correct typo in Obadiah abbreviation
</commit_message>
<xml_diff>
--- a/source/bible_book_metadata.xlsx
+++ b/source/bible_book_metadata.xlsx
@@ -325,7 +325,7 @@
     <t xml:space="preserve">Ob.</t>
   </si>
   <si>
-    <t xml:space="preserve">Obsd.</t>
+    <t xml:space="preserve">Obad.</t>
   </si>
   <si>
     <t xml:space="preserve">Jonah</t>
@@ -724,10 +724,10 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.09"/>

</xml_diff>